<commit_message>
Have all connectors for PCB
</commit_message>
<xml_diff>
--- a/Mega Shield I O Spacing and connections.xlsx
+++ b/Mega Shield I O Spacing and connections.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Mega Shield Exterior Connections</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>Library found?</t>
+  </si>
+  <si>
+    <t>^yes (Under RJ11)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -592,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -690,6 +699,11 @@
         <v>53</v>
       </c>
     </row>
+    <row r="9" spans="1:12">
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>7</v>
@@ -713,6 +727,9 @@
       <c r="G12">
         <v>5</v>
       </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
@@ -737,6 +754,9 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -761,6 +781,9 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
@@ -785,6 +808,9 @@
       <c r="G15">
         <v>1.4</v>
       </c>
+      <c r="H15" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
@@ -798,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -810,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -822,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -834,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -846,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -869,8 +895,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -882,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -891,13 +920,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -906,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -918,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -942,7 +971,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -950,8 +979,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -960,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -971,8 +1003,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -995,8 +1030,11 @@
       <c r="G31">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1008,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1031,8 +1069,11 @@
       <c r="G33">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1041,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1064,8 +1105,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -1088,8 +1132,11 @@
       <c r="G36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1112,8 +1159,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1125,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1137,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1160,8 +1210,11 @@
       <c r="G40">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1173,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -1185,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1197,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1218,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -1227,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1251,12 +1304,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>64</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
+      </c>
+      <c r="H48" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="7:7">

</xml_diff>